<commit_message>
Updated cross Browser test case
</commit_message>
<xml_diff>
--- a/Mobiquity_TestCases.xlsx
+++ b/Mobiquity_TestCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>Employee Lee_Updated Test_Updated should not be listed in the employee list on the home page.</t>
+  </si>
+  <si>
+    <t>Cross Browser Testing</t>
+  </si>
+  <si>
+    <t>Execute all the above scenarios on Chrome, Firefox, IE other browsers</t>
+  </si>
+  <si>
+    <t>Chrome, Firefox, IE,</t>
+  </si>
+  <si>
+    <t>Should run the tests in all the browsers without fail.</t>
   </si>
 </sst>
 </file>
@@ -282,11 +294,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -582,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -615,10 +627,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="45">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -635,8 +647,8 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
@@ -648,8 +660,8 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
@@ -661,8 +673,8 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
@@ -672,8 +684,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="6" t="s">
         <v>19</v>
       </c>
@@ -683,8 +695,8 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
@@ -696,8 +708,8 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
@@ -709,12 +721,12 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -722,12 +734,12 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -735,8 +747,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="30">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="6" t="s">
         <v>30</v>
       </c>
@@ -759,10 +771,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="30">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -776,8 +788,8 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="6" t="s">
         <v>26</v>
       </c>
@@ -789,8 +801,8 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
@@ -802,12 +814,12 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -815,12 +827,12 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -828,8 +840,8 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
@@ -839,8 +851,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="6" t="s">
         <v>34</v>
       </c>
@@ -852,10 +864,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="30">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -869,8 +881,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="4" t="s">
         <v>54</v>
       </c>
@@ -880,8 +892,8 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="6" t="s">
         <v>56</v>
       </c>
@@ -891,8 +903,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
@@ -902,25 +914,39 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>